<commit_message>
Milestone has been set newly.
Milestone has been set newly.
</commit_message>
<xml_diff>
--- a/dustbin/SpringHRM_Requirements_Final.xlsx
+++ b/dustbin/SpringHRM_Requirements_Final.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2099" uniqueCount="760">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2102" uniqueCount="763">
   <si>
     <t>Changes in Red</t>
   </si>
@@ -3840,6 +3840,15 @@
   </si>
   <si>
     <t>Milestone 5</t>
+  </si>
+  <si>
+    <t>Milestone 6</t>
+  </si>
+  <si>
+    <t>Milestone 7</t>
+  </si>
+  <si>
+    <t>Milestone 8</t>
   </si>
 </sst>
 </file>
@@ -12359,8 +12368,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K422"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="B106" sqref="B106"/>
+    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="E120" sqref="E120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -12376,7 +12385,7 @@
     <col min="11" max="11" width="27.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="133" customFormat="1">
+    <row r="1" spans="1:11" s="133" customFormat="1" ht="90">
       <c r="A1" s="131" t="s">
         <v>248</v>
       </c>
@@ -14057,7 +14066,9 @@
       <c r="B107" s="98"/>
       <c r="C107" s="47"/>
       <c r="D107" s="47"/>
-      <c r="E107" s="47"/>
+      <c r="E107" s="47" t="s">
+        <v>760</v>
+      </c>
       <c r="F107" s="47"/>
       <c r="G107" s="47"/>
       <c r="H107" s="47"/>
@@ -14132,7 +14143,9 @@
       <c r="B112" s="98"/>
       <c r="C112" s="47"/>
       <c r="D112" s="47"/>
-      <c r="E112" s="47"/>
+      <c r="E112" s="47" t="s">
+        <v>761</v>
+      </c>
       <c r="F112" s="47"/>
       <c r="G112" s="47"/>
       <c r="H112" s="47"/>
@@ -14237,7 +14250,9 @@
       <c r="B119" s="98"/>
       <c r="C119" s="47"/>
       <c r="D119" s="47"/>
-      <c r="E119" s="47"/>
+      <c r="E119" s="47" t="s">
+        <v>762</v>
+      </c>
       <c r="F119" s="47"/>
       <c r="G119" s="47"/>
       <c r="H119" s="47"/>

</xml_diff>